<commit_message>
Added additional data files and calibrations, changed file-refs to pycharm directory.
</commit_message>
<xml_diff>
--- a/Data/Calibrations.xlsx
+++ b/Data/Calibrations.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="16925"/>
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Acceleration\Digitized tracks\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kara\PycharmProjects\FishTrackProcessing\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="12180" windowHeight="4800"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="12180" windowHeight="4800" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="171027"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,18 +25,21 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="3">
   <si>
     <t>L</t>
   </si>
   <si>
     <t>V</t>
   </si>
+  <si>
+    <t>"y(cm/s) = 01411x(RPM) -1.7937"</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -161,6 +165,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -196,6 +217,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -350,7 +388,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
@@ -539,4 +577,24 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Added more trials and updated trial_info.csv
</commit_message>
<xml_diff>
--- a/Data/Calibrations.xlsx
+++ b/Data/Calibrations.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="12180" windowHeight="4800" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="12180" windowHeight="4800"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
     <t>V</t>
   </si>
   <si>
-    <t>"y(cm/s) = 01411x(RPM) -1.7937"</t>
+    <t>"y(cm/s) = 0.1411x(RPM) -1.7937"</t>
   </si>
 </sst>
 </file>
@@ -388,8 +388,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -583,8 +583,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>